<commit_message>
the link label is now a node representing a data object
</commit_message>
<xml_diff>
--- a/Group_A_TaskRisk_log.xlsx
+++ b/Group_A_TaskRisk_log.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D210209-8AA0-4DE8-B198-98286DD2E35B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190FE994-0ECF-4D47-BAE6-38D6CB970228}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="412" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="412" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -201,9 +201,6 @@
     <t>Programming difficulties (different skills in programming or less experience)</t>
   </si>
   <si>
-    <t>Last update: 28.04.2021</t>
-  </si>
-  <si>
     <t>A group member is getting ill or has to step back for longterm</t>
   </si>
   <si>
@@ -375,6 +372,9 @@
   </si>
   <si>
     <t>Being able to solve the export tasks</t>
+  </si>
+  <si>
+    <t>Last update: 24.05.2021</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -625,10 +625,19 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1019,8 +1028,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="A3:I33" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
-  <autoFilter ref="A3:I33" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="A3:I35" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+  <autoFilter ref="A3:I35" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Task" dataDxfId="19"/>
@@ -1343,38 +1352,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="117" customWidth="1"/>
-    <col min="3" max="3" width="88.140625" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="121" customWidth="1"/>
+    <col min="3" max="3" width="83.140625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" style="22" customWidth="1"/>
-    <col min="7" max="8" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" customWidth="1"/>
     <col min="11" max="11" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="25"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="29"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
@@ -1584,7 +1595,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>35</v>
@@ -1642,10 +1653,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>62</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>52</v>
@@ -1671,16 +1682,16 @@
         <v>10</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>34</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F13" s="20">
         <v>1</v>
@@ -1700,16 +1711,16 @@
         <v>11</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>34</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F14" s="20">
         <v>1</v>
@@ -1729,16 +1740,16 @@
         <v>12</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F15" s="20">
         <v>1</v>
@@ -1758,16 +1769,16 @@
         <v>13</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>31</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F16" s="20">
         <v>1</v>
@@ -1787,16 +1798,16 @@
         <v>14</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>24</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F17" s="20">
         <v>1</v>
@@ -1816,10 +1827,10 @@
         <v>15</v>
       </c>
       <c r="B18" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>85</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>86</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>31</v>
@@ -1845,16 +1856,16 @@
         <v>16</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>28</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F19" s="20">
         <v>1</v>
@@ -1874,16 +1885,16 @@
         <v>17</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>36</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F20" s="20">
         <v>1</v>
@@ -1903,10 +1914,10 @@
         <v>18</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>36</v>
@@ -1920,18 +1931,22 @@
       <c r="G21" s="14">
         <v>4</v>
       </c>
-      <c r="H21" s="13"/>
-      <c r="I21" s="14"/>
+      <c r="H21" s="13">
+        <v>2</v>
+      </c>
+      <c r="I21" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>19</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D22" s="13" t="s">
         <v>24</v>
@@ -1957,10 +1972,10 @@
         <v>20</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>34</v>
@@ -1982,10 +1997,10 @@
         <v>21</v>
       </c>
       <c r="B24" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" s="13" t="s">
         <v>103</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>104</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>36</v>
@@ -1999,18 +2014,22 @@
       <c r="G24" s="14">
         <v>2</v>
       </c>
-      <c r="H24" s="13"/>
-      <c r="I24" s="14"/>
+      <c r="H24" s="13">
+        <v>2</v>
+      </c>
+      <c r="I24" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>22</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>31</v>
@@ -2032,10 +2051,10 @@
         <v>23</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>31</v>
@@ -2057,10 +2076,10 @@
         <v>24</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>28</v>
@@ -2082,10 +2101,10 @@
         <v>25</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>28</v>
@@ -2107,10 +2126,10 @@
         <v>26</v>
       </c>
       <c r="B29" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="13" t="s">
         <v>112</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>113</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>34</v>
@@ -2132,10 +2151,10 @@
         <v>27</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D30" s="15" t="s">
         <v>34</v>
@@ -2157,10 +2176,10 @@
         <v>28</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>24</v>
@@ -2182,10 +2201,10 @@
         <v>29</v>
       </c>
       <c r="B32" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="13" t="s">
         <v>64</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>65</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>31</v>
@@ -2207,10 +2226,10 @@
         <v>30</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D33" s="13" t="s">
         <v>36</v>
@@ -2228,7 +2247,9 @@
       <c r="I33" s="14"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
+      <c r="A34" s="11">
+        <v>31</v>
+      </c>
       <c r="B34" s="12"/>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
@@ -2239,18 +2260,23 @@
       <c r="I34" s="14"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="14"/>
+      <c r="A35" s="24">
+        <v>32</v>
+      </c>
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="16"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G36" s="26"/>
+      <c r="G36" s="23"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I37" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2281,7 +2307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -2404,10 +2430,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>28</v>
@@ -2419,10 +2445,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>52</v>
@@ -2434,10 +2460,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Addet Task to Tasklog
</commit_message>
<xml_diff>
--- a/Group_A_TaskRisk_log.xlsx
+++ b/Group_A_TaskRisk_log.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05113CC4-06A6-9447-A888-FB78B8FCC05E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6052FD20-A1AD-0F40-B5F5-30601C55B2C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" tabRatio="412" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="500" windowWidth="38400" windowHeight="19920" tabRatio="412" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="128">
   <si>
     <t>#</t>
   </si>
@@ -405,6 +405,18 @@
   </si>
   <si>
     <t>Communication between app and database</t>
+  </si>
+  <si>
+    <t>Rename the Status to COTS Label</t>
+  </si>
+  <si>
+    <t>Make Data Object reusable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reusing an existing Data Object, attached to different line </t>
+  </si>
+  <si>
+    <t>Refactoring the Code</t>
   </si>
 </sst>
 </file>
@@ -593,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -661,6 +673,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1051,8 +1069,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="A3:I38" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
-  <autoFilter ref="A3:I38" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="A3:I41" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+  <autoFilter ref="A3:I41" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Task" dataDxfId="19"/>
@@ -1375,10 +1393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2437,6 +2455,57 @@
       </c>
       <c r="H38" s="15"/>
       <c r="I38" s="16"/>
+    </row>
+    <row r="39" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="27">
+        <v>36</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="28">
+        <v>3</v>
+      </c>
+      <c r="G39" s="16"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="16"/>
+    </row>
+    <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="27">
+        <v>37</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="28">
+        <v>3</v>
+      </c>
+      <c r="G40" s="16"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="16"/>
+    </row>
+    <row r="41" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="27">
+        <v>38</v>
+      </c>
+      <c r="B41" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>